<commit_message>
First draft of model for teaching Uni Brazilia
</commit_message>
<xml_diff>
--- a/data/hips_input_data.xlsx
+++ b/data/hips_input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/Teaching/EE using R/hips_teaching_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{932E4C0E-6096-432E-9AF8-9CBD919C620B}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{271CC3B1-3BDB-47C5-9962-84DA51C7B301}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log_rates_1st_revision" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -629,10 +629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AC2176-5E32-46C4-A5C4-2B7AFA8F2C2E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -640,7 +640,7 @@
     <col min="1" max="1" width="25.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -661,8 +661,12 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2">
+        <f>1-EXP(-EXP(B2))</f>
+        <v>4.2208728839985277E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -673,7 +677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -683,8 +687,12 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="L4">
+        <f t="shared" ref="L3:L4" si="0">1-EXP(-EXP(B4))</f>
+        <v>5.625775354315421E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -705,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6164E5D0-EE06-4E7F-BDB7-4D02683FEDD0}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Fixed error in xlsx file
</commit_message>
<xml_diff>
--- a/data/hips_input_data.xlsx
+++ b/data/hips_input_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/Teaching/EE using R/hips_teaching_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{271CC3B1-3BDB-47C5-9962-84DA51C7B301}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D31DC5-0CE7-4B02-AC5E-AAD284C075F0}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,10 +629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AC2176-5E32-46C4-A5C4-2B7AFA8F2C2E}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -640,7 +640,7 @@
     <col min="1" max="1" width="25.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -661,12 +661,8 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="L2">
-        <f>1-EXP(-EXP(B2))</f>
-        <v>4.2208728839985277E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -677,7 +673,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -687,12 +683,8 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L3:L4" si="0">1-EXP(-EXP(B4))</f>
-        <v>5.625775354315421E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>